<commit_message>
Working more on percent instruction
Former-commit-id: 826636f133b4bd1842a757419f955655b931ab36
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D83ADD5F-04C9-4B9A-BE1F-A6E00AFF92FF}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F802B2B4-6A5C-430F-99EF-2D17C8C88ED8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="0" yWindow="4395" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
+    <sheet name="VOCALS x 2" sheetId="2" r:id="rId2"/>
+    <sheet name="VOCALS x 10" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>ACTUAL</t>
   </si>
@@ -76,6 +78,18 @@
   </si>
   <si>
     <t>Using vocals.wav files after ran through spleeter</t>
+  </si>
+  <si>
+    <t>&gt;= 0 dB</t>
+  </si>
+  <si>
+    <t>Using video_#_vocals_x2.wav files after ran through spleeter and decibels * 2 in ffmpeg</t>
+  </si>
+  <si>
+    <t>Using video_#_vocals_x10.wav files after ran through spleeter and decibels * 2 in ffmpeg</t>
+  </si>
+  <si>
+    <t>0/0.1</t>
   </si>
 </sst>
 </file>
@@ -437,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7AD36-5A88-4CD6-B706-FB209ABF0E6E}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,9 +603,289 @@
         <v>0.49609999999999999</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.47849999999999998</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.50790000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.50229999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79095F3F-8D6B-4A54-BF89-FA6C4083D339}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.49990000000000001</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.1402000000000001</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.8192999999999999</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2044BF24-F3C3-4EAA-A0DC-BB89E6F1CBF2}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.5165999999999999</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Still working on manual audio labels
Former-commit-id: 2a5a54164efa86a8433525db76f0d3dcf8a85e87
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F802B2B4-6A5C-430F-99EF-2D17C8C88ED8}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9E78389A-BC82-4A62-A052-DD8079A31E6E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4395" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="0" yWindow="4815" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>ACTUAL</t>
   </si>
@@ -90,13 +90,16 @@
   </si>
   <si>
     <t>0/0.1</t>
+  </si>
+  <si>
+    <t>EDITED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +113,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,17 +143,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,9 +470,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7AD36-5A88-4CD6-B706-FB209ABF0E6E}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -487,133 +506,101 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.3301</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.1978</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.9294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.84950000000000003</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.6294999999999999</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.0045000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.4098999999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.35070000000000001</v>
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.45579999999999998</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.2442</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.29799999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.2535</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.33379999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>0.2442</v>
+        <v>0.43169999999999997</v>
       </c>
       <c r="C12" s="1">
-        <v>0.14660000000000001</v>
+        <v>0.4531</v>
       </c>
       <c r="D12" s="1">
-        <v>0.29799999999999999</v>
+        <v>0.46029999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>0.2535</v>
+        <v>0.441</v>
       </c>
       <c r="C13" s="1">
-        <v>0.14899999999999999</v>
+        <v>0.45550000000000002</v>
       </c>
       <c r="D13" s="1">
-        <v>0.33379999999999999</v>
+        <v>0.49609999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>0.43169999999999997</v>
+        <v>0.47849999999999998</v>
       </c>
       <c r="C14" s="1">
-        <v>0.4531</v>
+        <v>0.50790000000000002</v>
       </c>
       <c r="D14" s="1">
-        <v>0.46029999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.441</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.45550000000000002</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.49609999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.47849999999999998</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.50790000000000002</v>
-      </c>
-      <c r="D16" s="1">
         <v>0.50229999999999997</v>
       </c>
     </row>
@@ -628,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79095F3F-8D6B-4A54-BF89-FA6C4083D339}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaning the repository more, made NOTES sheet
Former-commit-id: 79b94958ce225b7dee75ded442edb2750aa615c6
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C7FFBB87-C608-4D73-8FBD-0299309306D0}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3A732C8E-D404-4880-AEA8-8B32CDDEB3AD}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="1950" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>ACTUAL</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>EDITED</t>
+  </si>
+  <si>
+    <t>Closest</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +518,23 @@
       <c r="C5" s="4">
         <v>0.57189999999999996</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="4">
+        <v>0.46260000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Added seconds of instruction to the percent of instruction sheet
Former-commit-id: 55c8ef4c363f5346d8736a7c933db4e9e946afd5
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3A732C8E-D404-4880-AEA8-8B32CDDEB3AD}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{655E6590-1860-4356-9637-80B837288678}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="17685" yWindow="6585" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>ACTUAL</t>
   </si>
@@ -95,7 +95,16 @@
     <t>EDITED</t>
   </si>
   <si>
-    <t>Closest</t>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>1060</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>Seconds, (0 dB - 80 dB)</t>
   </si>
 </sst>
 </file>
@@ -150,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -158,6 +167,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -473,15 +488,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7AD36-5A88-4CD6-B706-FB209ABF0E6E}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -527,13 +545,13 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>470</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>1331</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>789</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,12 +641,29 @@
       </c>
       <c r="D14" s="1">
         <v>0.50229999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6">
+        <v>455</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C16:D16" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added CK to instruction sheet
Former-commit-id: e592ba93a5ccde66f844e71270ef61b46bac608f
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{655E6590-1860-4356-9637-80B837288678}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B512C0EB-7753-4A82-B00B-2BFF8B30A8D1}"/>
   <bookViews>
-    <workbookView xWindow="17685" yWindow="6585" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="16740" yWindow="5835" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
-    <sheet name="VOCALS x 2" sheetId="2" r:id="rId2"/>
-    <sheet name="VOCALS x 10" sheetId="4" r:id="rId3"/>
+    <sheet name="Cohen's Kappa" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ACTUAL</t>
   </si>
@@ -50,18 +49,9 @@
     <t>VIDEO_3</t>
   </si>
   <si>
-    <t>1/0.1</t>
-  </si>
-  <si>
     <t>LABELS</t>
   </si>
   <si>
-    <t>8/0.1</t>
-  </si>
-  <si>
-    <t>10/0.1</t>
-  </si>
-  <si>
     <t>Percent_of_Instruction</t>
   </si>
   <si>
@@ -83,15 +73,6 @@
     <t>&gt;= 0 dB</t>
   </si>
   <si>
-    <t>Using video_#_vocals_x2.wav files after ran through spleeter and decibels * 2 in ffmpeg</t>
-  </si>
-  <si>
-    <t>Using video_#_vocals_x10.wav files after ran through spleeter and decibels * 2 in ffmpeg</t>
-  </si>
-  <si>
-    <t>0/0.1</t>
-  </si>
-  <si>
     <t>EDITED</t>
   </si>
   <si>
@@ -105,13 +86,61 @@
   </si>
   <si>
     <t>Seconds, (0 dB - 80 dB)</t>
+  </si>
+  <si>
+    <t>Actual not instructing</t>
+  </si>
+  <si>
+    <t>Actual instructing</t>
+  </si>
+  <si>
+    <t>dB detected instructing</t>
+  </si>
+  <si>
+    <t>dB not detected instructing</t>
+  </si>
+  <si>
+    <t>CK_Vid1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK </t>
+  </si>
+  <si>
+    <t>p(O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p(E) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p(Yes) </t>
+  </si>
+  <si>
+    <t>p(No)</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>CK_Vid2</t>
+  </si>
+  <si>
+    <t>CK_Vid3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +161,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,6 +215,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7AD36-5A88-4CD6-B706-FB209ABF0E6E}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,21 +549,24 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -526,9 +578,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4">
         <v>0.45579999999999998</v>
@@ -539,10 +591,11 @@
       <c r="D5" s="4">
         <v>0.46260000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>470</v>
@@ -554,14 +607,14 @@
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -573,9 +626,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>0.2442</v>
@@ -587,9 +640,9 @@
         <v>0.29799999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>0.2535</v>
@@ -601,9 +654,9 @@
         <v>0.33379999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>0.43169999999999997</v>
@@ -615,9 +668,9 @@
         <v>0.46029999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1">
         <v>0.441</v>
@@ -629,9 +682,9 @@
         <v>0.49609999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>0.47849999999999998</v>
@@ -643,18 +696,43 @@
         <v>0.50229999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B16" s="6">
         <v>455</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>0.97060000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.77012800000000003</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.92908999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -668,265 +746,367 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79095F3F-8D6B-4A54-BF89-FA6C4083D339}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313EF0B3-A87E-4E3F-B571-0E82439A5742}">
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7">
+        <v>561</v>
+      </c>
+      <c r="C2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
+      <c r="C3">
+        <v>455</v>
+      </c>
+      <c r="D3">
+        <v>455</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
+      <c r="A4" s="2"/>
+      <c r="B4">
+        <v>561</v>
+      </c>
+      <c r="C4">
+        <v>470</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.49990000000000001</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.1402000000000001</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <f>(B2+C3)/(B2+C2+B3+C3)</f>
+        <v>0.98545101842870997</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.8192999999999999</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f>(B2+C2)/(B2+C2+B3+C3)</f>
+        <v>0.55868089233753637</v>
+      </c>
+      <c r="C8">
+        <f>(B2+B3)/(B2+C2+B3+C3)</f>
+        <v>0.54413191076624634</v>
+      </c>
+      <c r="D8">
+        <f>B8*C8</f>
+        <v>0.3039961014562152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <f>(B3+C3)/(B2+C2+B3+C3)</f>
+        <v>0.44131910766246363</v>
+      </c>
+      <c r="C9">
+        <f>(C2+C3)/(C2+C3+B3+B2)</f>
+        <v>0.45586808923375366</v>
+      </c>
+      <c r="D9">
+        <f>B9*C9</f>
+        <v>0.20118329835243251</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <f>D8+D9</f>
+        <v>0.50517939980864768</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <f>(B6-B10)/(1-B10)</f>
+        <v>0.97059746185655205</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="7">
+        <v>997</v>
+      </c>
+      <c r="C14">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1060</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2044BF24-F3C3-4EAA-A0DC-BB89E6F1CBF2}">
-  <dimension ref="A1:D17"/>
-  <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <f>(B14+C15)/(B14+C14+B15+C15)</f>
+        <v>0.88359106529209619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <f>(B14+C14)/(B14+C14+B15+C15)</f>
+        <v>0.5446735395189003</v>
+      </c>
+      <c r="C20">
+        <f>(B14+B15)/(B14+C14+B15+C15)</f>
+        <v>0.42826460481099654</v>
+      </c>
+      <c r="D20">
+        <f>B20*C20</f>
+        <v>0.23326439815306854</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f>(B15+C15)/(B14+C14+B15+C15)</f>
+        <v>0.45532646048109965</v>
+      </c>
+      <c r="C21">
+        <f>(C14+C15)/(C14+C15+B15+B14)</f>
+        <v>0.5717353951890034</v>
+      </c>
+      <c r="D21">
+        <f>B21*C21</f>
+        <v>0.26032625382317165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <f>D20+D21</f>
+        <v>0.49359065197624019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>(B18-B22)/(1-B22)</f>
+        <v>0.77012877988492001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="7">
+        <v>914</v>
+      </c>
+      <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.749</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.5165999999999999</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <f>(B26+C27)/(B26+C26+B27+C27)</f>
+        <v>0.96453900709219853</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <f>(B26+C26)/(B26+C26+B27+C27)</f>
+        <v>0.49863611565739224</v>
+      </c>
+      <c r="C32">
+        <f>(B26+B27)/(B26+C26+B27+C27)</f>
+        <v>0.53409710856519366</v>
+      </c>
+      <c r="D32">
+        <f>B32*C32</f>
+        <v>0.26632010759879271</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <f>(B27+C27)/(B26+C26+B27+C27)</f>
+        <v>0.5013638843426077</v>
+      </c>
+      <c r="C33">
+        <f>(C26+C27)/(C26+C27+B27+B26)</f>
+        <v>0.46590289143480634</v>
+      </c>
+      <c r="D33">
+        <f>B33*C33</f>
+        <v>0.23358688337620676</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <f>D32+D33</f>
+        <v>0.49990699097499947</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <f>(B30-B34)/(1-B34)</f>
+        <v>0.92909120450026383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added table of contents
Former-commit-id: 3c06ca0471818101ad1c9f7cf4b48f9bab391d89
</commit_message>
<xml_diff>
--- a/3 Beginner Videos/Percentage_of_Instruction.xlsx
+++ b/3 Beginner Videos/Percentage_of_Instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/3 Beginner Videos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B512C0EB-7753-4A82-B00B-2BFF8B30A8D1}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{0B93AD97-20E7-4D8D-B413-CB33A71E6C22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{43B5CD3A-C25F-4197-9AFF-F22E6CD029EE}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="5835" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
+    <workbookView xWindow="7200" yWindow="4815" windowWidth="21600" windowHeight="11385" xr2:uid="{F8DC8BCC-F4F8-443A-80F4-F184F88EE57D}"/>
   </bookViews>
   <sheets>
     <sheet name="VOCALS" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7AD36-5A88-4CD6-B706-FB209ABF0E6E}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,9 +711,6 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -725,6 +722,9 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="1">
         <v>0.97060000000000002</v>
       </c>

</xml_diff>